<commit_message>
Adding some processing code
</commit_message>
<xml_diff>
--- a/Recipe Recommendation Machine Learning/Created Data Example-Dictionary.xlsx
+++ b/Recipe Recommendation Machine Learning/Created Data Example-Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomascartotto/Desktop/CannJoin_MMAI/Recipe Recommendation Machine Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD24C9F8-7FAB-D542-90E1-4244DD296353}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3478B2-8D42-7949-AB7E-F5FB9EDB6C71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4340" yWindow="-21140" windowWidth="25600" windowHeight="21140" activeTab="1" xr2:uid="{6A0FF0BD-9552-C444-AC61-2306B75588B9}"/>
+    <workbookView xWindow="2640" yWindow="480" windowWidth="25600" windowHeight="19500" activeTab="1" xr2:uid="{6A0FF0BD-9552-C444-AC61-2306B75588B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>Uses Butter (1 or 0)</t>
   </si>
@@ -170,9 +170,6 @@
     <t>What symptom they are trying to help (Categorical)</t>
   </si>
   <si>
-    <t>Did this weed/recipe mixture provide relief (True False)</t>
-  </si>
-  <si>
     <t>Customer Generated</t>
   </si>
   <si>
@@ -219,13 +216,62 @@
   </si>
   <si>
     <t>Stress</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>The original comment on the review</t>
+  </si>
+  <si>
+    <t>commnet_polarity</t>
+  </si>
+  <si>
+    <t>comment_subjectivity</t>
+  </si>
+  <si>
+    <t>DATA DICTIONARY USER REVIEW</t>
+  </si>
+  <si>
+    <t>DATA DICTIONARY STRAIN</t>
+  </si>
+  <si>
+    <t>DATA DICTIONARY RECIPE</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>The comment's polarity (used to calculate strain average polarity)</t>
+  </si>
+  <si>
+    <t>The comments Subjectivity  (used to calculate strain average Subjectivity)</t>
+  </si>
+  <si>
+    <t>The comments Rating  (used to calculate strain average  Rating)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Did this weed/recipe mixture provide relief (True False) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TARGET ATTRIBUTE</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -236,6 +282,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -280,13 +333,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,312 +782,345 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB124B7D-4A61-EC45-B317-89C34BDE336F}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.1640625" customWidth="1"/>
+    <col min="2" max="2" width="75.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:16" ht="24">
+      <c r="A1" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="F2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>27</v>
+      <c r="A8" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>47</v>
+      <c r="F15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7">
-      <c r="F17" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="6:7">
-      <c r="F18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="6:7">
-      <c r="F19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="6:7">
-      <c r="F20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="6:7">
-      <c r="F21" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="6:7">
-      <c r="F22" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="6:7">
-      <c r="F23" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="6:7">
-      <c r="F24" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="6:7">
-      <c r="F25" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="6:7">
-      <c r="F26" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="6:7">
-      <c r="F27" t="s">
-        <v>59</v>
-      </c>
-      <c r="G27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="6:7">
-      <c r="F28" t="s">
-        <v>60</v>
-      </c>
-      <c r="G28">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="6:7">
-      <c r="F29" t="s">
-        <v>61</v>
-      </c>
-      <c r="G29">
-        <v>14</v>
+    </row>
+    <row r="24" spans="1:3" ht="24">
+      <c r="A24" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="24">
+      <c r="A38" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>